<commit_message>
Added InstituteOnBoardingRegistrationPageObjects.java , InstituteOnBoardingRegistrationPage_Test , InstituteOnBoardingRegistration_TestData.xlsx , Wrote script for On boarding registration page for Institution,
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/AllCredsLogins_TestData.xlsx
+++ b/src/test/resources/testData/AllCredsLogins_TestData.xlsx
@@ -1,26 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="330" windowWidth="15300" windowHeight="2760"/>
+    <workbookView windowWidth="12888" windowHeight="4872"/>
   </bookViews>
   <sheets>
     <sheet name="AllRoleLogins" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="144525"/>
+  <oleSize ref="A1:E4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>TC No</t>
   </si>
@@ -28,9 +24,57 @@
     <t>TC Name</t>
   </si>
   <si>
+    <t>Role</t>
+  </si>
+  <si>
     <t>username</t>
   </si>
   <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>Verify able to login as Admin</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>hr@snipe.co.in</t>
+  </si>
+  <si>
+    <t>Admin123</t>
+  </si>
+  <si>
+    <t>Verify able to login as Institute</t>
+  </si>
+  <si>
+    <t>Institute</t>
+  </si>
+  <si>
+    <t>test2@gmail.com</t>
+  </si>
+  <si>
+    <t>welcome@123</t>
+  </si>
+  <si>
+    <t>Verify able to login as Faculty</t>
+  </si>
+  <si>
+    <t>Faculty</t>
+  </si>
+  <si>
+    <t>test3@gmail.com</t>
+  </si>
+  <si>
+    <t>Verify able to login as Student</t>
+  </si>
+  <si>
+    <t>Student</t>
+  </si>
+  <si>
+    <t>test1@gmail.com</t>
+  </si>
+  <si>
     <t>pass</t>
   </si>
   <si>
@@ -44,57 +88,24 @@
   </si>
   <si>
     <t>pass2</t>
-  </si>
-  <si>
-    <t>Admin</t>
-  </si>
-  <si>
-    <t>hr@snipe.co.in</t>
-  </si>
-  <si>
-    <t>Admin123</t>
-  </si>
-  <si>
-    <t>Institute</t>
-  </si>
-  <si>
-    <t>Faculty</t>
-  </si>
-  <si>
-    <t>test2@gmail.com</t>
-  </si>
-  <si>
-    <t>welcome@123</t>
-  </si>
-  <si>
-    <t>test3@gmail.com</t>
-  </si>
-  <si>
-    <t>Verify able to login as Admin</t>
-  </si>
-  <si>
-    <t>Verify able to login as Institute</t>
-  </si>
-  <si>
-    <t>Verify able to login as Faculty</t>
-  </si>
-  <si>
-    <t>Role</t>
-  </si>
-  <si>
-    <t>password</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -102,17 +113,161 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -125,8 +280,194 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -136,39 +477,325 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
+    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
+    <cellStyle name="Note" xfId="12" builtinId="10"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -250,23 +877,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -302,23 +912,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -460,32 +1053,27 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="4" outlineLevelCol="4"/>
   <cols>
-    <col min="2" max="2" width="41.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.5740740740741" customWidth="1"/>
+    <col min="3" max="3" width="12.287037037037" customWidth="1"/>
+    <col min="4" max="4" width="13.712962962963" customWidth="1"/>
+    <col min="5" max="5" width="22.5740740740741" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -493,107 +1081,131 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>10</v>
-      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="E3" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D5" r:id="rId1" display="test1@gmail.com"/>
+    <hyperlink ref="E5" r:id="rId2" display="welcome@123"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="1" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="2" outlineLevelCol="1"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Refactored code Wrote test for log in as institute after successful on board registration
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/AllCredsLogins_TestData.xlsx
+++ b/src/test/resources/testData/AllCredsLogins_TestData.xlsx
@@ -4,19 +4,18 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="12888" windowHeight="4872"/>
+    <workbookView windowWidth="22368" windowHeight="9215"/>
   </bookViews>
   <sheets>
     <sheet name="AllRoleLogins" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
-  <oleSize ref="A1:E4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
   <si>
     <t>TC No</t>
   </si>
@@ -73,6 +72,15 @@
   </si>
   <si>
     <t>test1@gmail.com</t>
+  </si>
+  <si>
+    <t>Verify Able to Login As Institute after Onboarding Registration</t>
+  </si>
+  <si>
+    <t>vedant.institute234@gmail.com</t>
+  </si>
+  <si>
+    <t>welcome123</t>
   </si>
   <si>
     <t>pass</t>
@@ -95,12 +103,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -117,10 +125,111 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -131,68 +240,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -202,68 +266,6 @@
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -282,13 +284,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -300,55 +434,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -361,108 +465,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -491,10 +493,27 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -515,41 +534,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -561,6 +545,24 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -583,163 +585,162 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="32" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1059,17 +1060,17 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="4" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="5" outlineLevelCol="4"/>
   <cols>
-    <col min="2" max="2" width="41.5740740740741" customWidth="1"/>
+    <col min="2" max="2" width="61.4351851851852" customWidth="1"/>
     <col min="3" max="3" width="12.287037037037" customWidth="1"/>
-    <col min="4" max="4" width="13.712962962963" customWidth="1"/>
+    <col min="4" max="4" width="33.7222222222222" customWidth="1"/>
     <col min="5" max="5" width="22.5740740740741" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1100,10 +1101,10 @@
       <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1117,10 +1118,10 @@
       <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1134,10 +1135,10 @@
       <c r="C4" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1151,11 +1152,28 @@
       <c r="C5" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1185,23 +1203,23 @@
         <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Create new faculty in institute and log in as Faculty
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/AllCredsLogins_TestData.xlsx
+++ b/src/test/resources/testData/AllCredsLogins_TestData.xlsx
@@ -4,18 +4,18 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22368" windowHeight="9215"/>
+    <workbookView windowWidth="22368" windowHeight="9215" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="AllRoleLogins" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Onboard_New_Institute" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="40">
   <si>
     <t>TC No</t>
   </si>
@@ -83,19 +83,58 @@
     <t>welcome123</t>
   </si>
   <si>
-    <t>pass</t>
-  </si>
-  <si>
-    <t>user1</t>
-  </si>
-  <si>
-    <t>pass1</t>
-  </si>
-  <si>
-    <t>user2</t>
-  </si>
-  <si>
-    <t>pass2</t>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>PhoneNumber</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>BioGraphy</t>
+  </si>
+  <si>
+    <t>Occupation</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>ConfirmPassword</t>
+  </si>
+  <si>
+    <t>Role_Faculty</t>
+  </si>
+  <si>
+    <t>Username_Faculty</t>
+  </si>
+  <si>
+    <t>Password_Faculty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Robert </t>
+  </si>
+  <si>
+    <t>Physics</t>
+  </si>
+  <si>
+    <t>robert123@gmail.com</t>
+  </si>
+  <si>
+    <t>Karnataka</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>Lecturer</t>
   </si>
 </sst>
 </file>
@@ -105,8 +144,8 @@
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -125,6 +164,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -132,56 +186,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -210,20 +232,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -240,6 +248,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
@@ -248,6 +264,21 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -256,14 +287,22 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -284,6 +323,66 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -296,7 +395,91 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -308,163 +491,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -493,6 +532,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -508,17 +556,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -530,21 +567,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -568,6 +590,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -584,24 +621,26 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -611,136 +650,139 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="32" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="7" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1062,8 +1104,8 @@
   <sheetPr/>
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="5" outlineLevelCol="4"/>
@@ -1190,39 +1232,130 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="2" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1"/>
+  <cols>
+    <col min="2" max="2" width="29.8888888888889" customWidth="1"/>
+    <col min="3" max="3" width="12.4444444444444" customWidth="1"/>
+    <col min="4" max="4" width="10.5555555555556" customWidth="1"/>
+    <col min="6" max="6" width="19.2222222222222" customWidth="1"/>
+    <col min="7" max="7" width="14.5555555555556" customWidth="1"/>
+    <col min="8" max="8" width="9.88888888888889" customWidth="1"/>
+    <col min="9" max="9" width="10.5555555555556" customWidth="1"/>
+    <col min="10" max="10" width="11.5555555555556" customWidth="1"/>
+    <col min="11" max="11" width="12.4444444444444" customWidth="1"/>
+    <col min="12" max="12" width="17.2222222222222" customWidth="1"/>
+    <col min="13" max="13" width="12.6666666666667" customWidth="1"/>
+    <col min="14" max="14" width="21.2222222222222" customWidth="1"/>
+    <col min="15" max="15" width="17.5555555555556" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:15">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>33</v>
+      </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:15">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" t="s">
-        <v>26</v>
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2">
+        <v>9876456789</v>
+      </c>
+      <c r="H2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J2" t="s">
+        <v>39</v>
+      </c>
+      <c r="K2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" t="s">
+        <v>21</v>
+      </c>
+      <c r="M2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="O2" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1" display="9876456789"/>
+    <hyperlink ref="E2" r:id="rId2" display="Physics" tooltip="mailto:vedant.institute234@gmail.com"/>
+    <hyperlink ref="N2" r:id="rId3" display="robert123@gmail.com"/>
+    <hyperlink ref="F2" r:id="rId3" display="robert123@gmail.com"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>

</xml_diff>